<commit_message>
Updated Growth and Real Estate
</commit_message>
<xml_diff>
--- a/Growth/GRAB_MODEL.xlsx
+++ b/Growth/GRAB_MODEL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Models\Growth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD56C76B-3DD9-4912-97CE-91207E14BAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65EC0A8-35A6-4527-B71D-1636E906C8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="4" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
   <si>
     <t>Price</t>
   </si>
@@ -472,15 +472,37 @@
     <t>Adjusted EBITDA 460-480:</t>
   </si>
   <si>
-    <t>Guidance unchanged</t>
+    <t>Upped Guidance 3.38 to 3.40 billion</t>
+  </si>
+  <si>
+    <t>490 to 500 mill adjusted ebitda</t>
+  </si>
+  <si>
+    <t>P/Sales</t>
+  </si>
+  <si>
+    <t>P/Book</t>
+  </si>
+  <si>
+    <t>EV/EBITDA</t>
+  </si>
+  <si>
+    <t>EV/R</t>
+  </si>
+  <si>
+    <t>Trailing P/E</t>
+  </si>
+  <si>
+    <t>Forward P/E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -493,12 +515,10 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -547,10 +567,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -572,6 +588,13 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -692,47 +715,52 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1211,102 +1239,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB11C10-986F-41A4-B3DD-2A72A923BC11}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="15">
         <v>5.34</v>
       </c>
-      <c r="C4" s="1">
-        <v>45858</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C4" s="16">
+        <v>45987</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="15">
         <v>4000</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C5" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="15">
         <f xml:space="preserve"> B4 * B5</f>
         <v>21360</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="15">
         <v>7600</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="15">
         <v>1888</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="15">
         <v>1.49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="15">
         <f>B6 - B7 + B8</f>
         <v>15648</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="15">
         <v>1.57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="15">
+        <v>6.63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="15">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="15">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="15">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1319,1611 +1396,1682 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E38C8F-3B6A-4584-925C-61BD108C4B76}">
   <dimension ref="A1:AD71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="13.140625" customWidth="1"/>
-    <col min="19" max="19" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="15"/>
+    <col min="2" max="2" width="23.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="9.140625" style="15"/>
+    <col min="15" max="18" width="13.140625" style="15" customWidth="1"/>
+    <col min="19" max="19" width="29.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.5703125" style="15" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" style="15" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="W2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="X2" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
         <v>3644</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>3878</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>4038</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>4501</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>4805</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>5055</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <v>5080</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="2">
         <v>4997</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
         <v>3600</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="15">
         <v>3939</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="15">
         <v>4063</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="15">
         <v>4183</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="15">
         <v>4242</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="15">
         <v>4434</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="15">
         <v>4659</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="15">
         <v>5028</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="15">
         <v>4932</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="15">
         <v>5354</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="V3" s="15">
+        <v>5774</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
         <v>28</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>29.1</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>25.9</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>29.6</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>30.9</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>32.6</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>33.5</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>33.6</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>33.299999999999997</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="15">
         <v>34.9</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="15">
         <v>36</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="15">
         <v>37.700000000000003</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="15">
         <v>38.5</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="15">
         <v>40.9</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="15">
         <v>41.9</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="15">
         <v>43.9</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="15">
         <v>44.5</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="15">
         <v>46.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="V4" s="15">
+        <v>47.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
         <v>130</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>133</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>156</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>152</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>155</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>155</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>151</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>149</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>125</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="15">
         <v>128</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="15">
         <v>128</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="15">
         <v>125</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="15">
         <v>123</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="15">
         <v>121</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="15">
         <v>124</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="15">
         <v>126</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="15">
         <v>122</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="15">
         <v>127</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
+      <c r="V5" s="15">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
         <v>139</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>172</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>187</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>218</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>216</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>212</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>199</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <v>174</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="2">
         <v>169</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="15">
         <v>175</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="15">
         <v>165</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="15">
         <v>172</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="15">
         <v>177</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="15">
         <v>186</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="15">
         <v>187</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="15">
         <v>204</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="15">
         <v>215</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="15">
         <v>239</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+      <c r="V6" s="15">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
         <v>186</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>243</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>271</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>365</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>344</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>311</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>277</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <v>238</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>222</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="15">
         <v>245</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="15">
         <v>216</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="15">
         <v>225</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="15">
         <v>239</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="15">
         <v>266</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="15">
         <v>275</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="15">
         <v>308</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="15">
         <v>286</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="15">
         <v>307</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
+      <c r="V7" s="15">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>0</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>0</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>0</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>0</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>0</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="2">
         <v>0</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="2">
         <v>196</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="15">
         <v>233</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="15">
         <v>275</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="15">
         <v>326</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="15">
         <v>363</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="15">
         <v>397</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="15">
         <v>498</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="15">
         <v>536</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="15">
         <v>566</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="15">
         <v>708</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
+      <c r="V8" s="15">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
         <v>53</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>45</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>49</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>1</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>91</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>134</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>171</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="2">
         <v>268</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="2">
         <v>294</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="15">
         <v>320</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="15">
         <v>335</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="15">
         <v>362</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="15">
         <v>350</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="15">
         <v>356</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="15">
         <v>380</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="15">
         <v>407</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="15">
         <v>415</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="15">
         <v>439</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
+      <c r="V10" s="15">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
         <v>145</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>118</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>88</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>106</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>112</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>161</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>176</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="2">
         <v>189</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="2">
         <v>194</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="15">
         <v>208</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="15">
         <v>231</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="15">
         <v>237</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="15">
         <v>247</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="15">
         <v>247</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="15">
         <v>271</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="15">
         <v>282</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="15">
         <v>282</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="15">
         <v>295</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
+      <c r="V11" s="15">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
         <v>8</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>6</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>14</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>-1</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>11</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>13</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>20</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="2">
         <v>28</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="2">
         <v>36</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="15">
         <v>39</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="15">
         <v>48</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="15">
         <v>54</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="15">
         <v>55</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="15">
         <v>60</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="15">
         <v>64</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="15">
         <v>74</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="15">
         <v>75</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="15">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="17" t="s">
+      <c r="V12" s="15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="12">
+      <c r="C13" s="9"/>
+      <c r="D13" s="17">
         <v>216</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="17">
         <v>179</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="17">
         <v>157</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="17">
         <v>122</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="17">
         <v>228</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="17">
         <v>321</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="17">
         <v>382</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="17">
         <v>502</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="17">
         <v>525</v>
       </c>
-      <c r="M13" s="12">
+      <c r="M13" s="17">
         <v>567</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="17">
         <v>615</v>
       </c>
-      <c r="O13" s="12">
+      <c r="O13" s="17">
         <v>653</v>
       </c>
-      <c r="P13" s="12">
+      <c r="P13" s="17">
         <v>653</v>
       </c>
-      <c r="Q13" s="12">
+      <c r="Q13" s="17">
         <v>664</v>
       </c>
-      <c r="R13" s="12">
+      <c r="R13" s="17">
         <v>716</v>
       </c>
-      <c r="S13" s="12">
+      <c r="S13" s="17">
         <v>764</v>
       </c>
-      <c r="T13" s="12">
+      <c r="T13" s="17">
         <v>773</v>
       </c>
-      <c r="U13" s="36">
+      <c r="U13" s="18">
         <v>819</v>
       </c>
-      <c r="V13" s="23">
-        <f t="shared" ref="U13:W13" si="0" xml:space="preserve"> U13 * 1.05</f>
-        <v>859.95</v>
-      </c>
-      <c r="W13" s="23">
-        <f t="shared" si="0"/>
-        <v>902.9475000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
+      <c r="V13" s="19">
+        <v>873</v>
+      </c>
+      <c r="W13" s="19">
+        <f t="shared" ref="W13" si="0" xml:space="preserve"> V13 * 1.05</f>
+        <v>916.65000000000009</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
         <v>6</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>10</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>3</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <v>0</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>3</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>3</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <v>3</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="2">
         <v>0</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="2">
         <v>3</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="15">
         <v>3</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="15">
         <v>6</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="15">
         <v>5</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="15">
         <v>2</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="15">
         <v>4</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="15">
         <v>6</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="15">
         <v>5</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="15">
         <v>8</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="15">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3" t="s">
+      <c r="V14" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="9">
+      <c r="C15" s="2"/>
+      <c r="D15" s="8">
         <v>241</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>266</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>266</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <v>298</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <v>310</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="8">
         <v>337</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="8">
         <v>321</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="8">
         <v>388</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="8">
         <v>372</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="8">
         <v>376</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="8">
         <v>375</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="15">
         <v>377</v>
       </c>
-      <c r="P15" s="9">
+      <c r="P15" s="8">
         <v>394</v>
       </c>
-      <c r="Q15" s="11">
+      <c r="Q15" s="8">
         <v>338</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="15">
         <v>409</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="15">
         <v>432</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="15">
         <v>449</v>
       </c>
-      <c r="U15">
+      <c r="U15" s="15">
         <v>465</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="17" t="s">
+      <c r="V15" s="15">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="17">
         <f t="shared" ref="C16:S16" si="1">C13 + C14 -C15</f>
         <v>0</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="17">
         <f t="shared" si="1"/>
         <v>-19</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="17">
         <f t="shared" si="1"/>
         <v>-77</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="17">
         <f t="shared" si="1"/>
         <v>-106</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="17">
         <f t="shared" si="1"/>
         <v>-176</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="17">
         <f t="shared" si="1"/>
         <v>-79</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="17">
         <f t="shared" si="1"/>
         <v>-13</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="17">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="17">
         <f t="shared" si="1"/>
         <v>114</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="17">
         <f t="shared" si="1"/>
         <v>156</v>
       </c>
-      <c r="M16" s="12">
+      <c r="M16" s="17">
         <f t="shared" si="1"/>
         <v>194</v>
       </c>
-      <c r="N16" s="12">
+      <c r="N16" s="17">
         <f t="shared" si="1"/>
         <v>246</v>
       </c>
-      <c r="O16" s="12">
+      <c r="O16" s="17">
         <f t="shared" si="1"/>
         <v>281</v>
       </c>
-      <c r="P16" s="12">
+      <c r="P16" s="17">
         <f t="shared" si="1"/>
         <v>261</v>
       </c>
-      <c r="Q16" s="12">
+      <c r="Q16" s="17">
         <f t="shared" si="1"/>
         <v>330</v>
       </c>
-      <c r="R16" s="12">
+      <c r="R16" s="17">
         <f t="shared" si="1"/>
         <v>313</v>
       </c>
-      <c r="S16" s="12">
+      <c r="S16" s="17">
         <f t="shared" si="1"/>
         <v>337</v>
       </c>
-      <c r="T16" s="12">
+      <c r="T16" s="17">
         <f>T13 + T14 -T15</f>
         <v>332</v>
       </c>
-      <c r="U16" s="12">
+      <c r="U16" s="17">
         <f>U13 + U14 -U15</f>
         <v>362</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
+      <c r="V16" s="17">
+        <f>V13 + V14 -V15</f>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="11">
+      <c r="C17" s="2"/>
+      <c r="D17" s="8">
         <v>45</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="8">
         <v>60</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="8">
         <v>51</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="8">
         <v>84</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="8">
         <v>70</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="8">
         <v>72</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="8">
         <v>66</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="8">
         <v>70</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="8">
         <v>70</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="8">
         <v>63</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="8">
         <v>76</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="8">
         <v>84</v>
       </c>
-      <c r="P17" s="11">
+      <c r="P17" s="8">
         <v>71</v>
       </c>
-      <c r="Q17" s="11">
+      <c r="Q17" s="8">
         <v>79</v>
       </c>
-      <c r="R17" s="11">
+      <c r="R17" s="8">
         <v>82</v>
       </c>
-      <c r="S17" s="11">
+      <c r="S17" s="8">
         <v>93</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="15">
         <v>82</v>
       </c>
-      <c r="U17" s="11">
+      <c r="U17" s="8">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
+      <c r="V17" s="8">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="11">
+      <c r="C18" s="2"/>
+      <c r="D18" s="8">
         <v>89</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="8">
         <v>154</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="8">
         <v>152</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="8">
         <v>176</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="8">
         <v>169</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="8">
         <v>162</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="8">
         <v>150</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="8">
         <v>166</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="8">
         <v>147</v>
       </c>
-      <c r="M18" s="11">
+      <c r="M18" s="8">
         <v>137</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="8">
         <v>131</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="15">
         <v>136</v>
       </c>
-      <c r="P18" s="11">
+      <c r="P18" s="8">
         <v>127</v>
       </c>
-      <c r="Q18" s="11">
+      <c r="Q18" s="8">
         <v>130</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="15">
         <v>112</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="15">
         <v>142</v>
       </c>
-      <c r="T18">
+      <c r="T18" s="15">
         <v>113</v>
       </c>
-      <c r="U18">
+      <c r="U18" s="15">
         <v>118</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3" t="s">
+      <c r="V18" s="15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="11">
+      <c r="C19" s="2"/>
+      <c r="D19" s="8">
         <v>75</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="8">
         <v>91</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="8">
         <v>93</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="8">
         <v>95</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="8">
         <v>119</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="8">
         <v>121</v>
       </c>
-      <c r="J19" s="11">
+      <c r="J19" s="8">
         <v>116</v>
       </c>
-      <c r="K19" s="11">
+      <c r="K19" s="8">
         <v>110</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="8">
         <v>128</v>
       </c>
-      <c r="M19" s="11">
+      <c r="M19" s="8">
         <v>91</v>
       </c>
-      <c r="N19" s="11">
+      <c r="N19" s="8">
         <v>99</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="15">
         <v>103</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="15">
         <v>116</v>
       </c>
-      <c r="Q19" s="11">
+      <c r="Q19" s="8">
         <v>104</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="15">
         <v>97</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="15">
         <v>93</v>
       </c>
-      <c r="T19">
+      <c r="T19" s="15">
         <v>121</v>
       </c>
-      <c r="U19">
+      <c r="U19" s="15">
         <v>113</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
+      <c r="V19" s="15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="11">
+      <c r="C20" s="2"/>
+      <c r="D20" s="8">
         <v>3</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="8">
         <v>7</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="8">
         <v>-2</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="8">
         <v>11</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="8">
         <v>8</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="8">
         <v>15</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="8">
         <v>17</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="8">
         <v>19</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="8">
         <v>13</v>
       </c>
-      <c r="M20" s="11">
+      <c r="M20" s="8">
         <v>20</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="8">
         <v>18</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="15">
         <v>21</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="15">
         <v>20</v>
       </c>
-      <c r="Q20" s="11">
+      <c r="Q20" s="8">
         <v>20</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="15">
         <v>19</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="15">
         <v>36</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="15">
         <v>33</v>
       </c>
-      <c r="U20">
+      <c r="U20" s="15">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3" t="s">
+      <c r="V20" s="15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="11">
+      <c r="C21" s="2"/>
+      <c r="D21" s="8">
         <v>0</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="8">
         <v>0</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F21" s="8">
         <v>1</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="8">
         <v>15</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H21" s="8">
         <v>0</v>
       </c>
-      <c r="I21" s="11">
+      <c r="I21" s="8">
         <v>1</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J21" s="8">
         <v>5</v>
       </c>
-      <c r="K21" s="11">
+      <c r="K21" s="8">
         <v>4</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L21" s="8">
         <v>2</v>
       </c>
-      <c r="M21" s="11">
+      <c r="M21" s="8">
         <v>59</v>
       </c>
-      <c r="N21" s="11">
+      <c r="N21" s="8">
         <v>15</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="15">
         <v>-17</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="15">
         <v>2</v>
       </c>
-      <c r="Q21" s="11">
+      <c r="Q21" s="8">
         <v>3</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="15">
         <v>41</v>
       </c>
-      <c r="S21">
+      <c r="S21" s="15">
         <v>-31</v>
       </c>
-      <c r="T21">
+      <c r="T21" s="15">
         <v>4</v>
       </c>
-      <c r="U21">
+      <c r="U21" s="15">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="17" t="s">
+      <c r="V21" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="17">
         <f t="shared" ref="C22:S22" si="2">C16-SUM(C17:C21)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="17">
         <f t="shared" si="2"/>
         <v>-231</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="17">
         <f t="shared" si="2"/>
         <v>-389</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="17">
         <f t="shared" si="2"/>
         <v>-401</v>
       </c>
-      <c r="G22" s="12">
+      <c r="G22" s="17">
         <f t="shared" si="2"/>
         <v>-557</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="17">
         <f t="shared" si="2"/>
         <v>-445</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="17">
         <f t="shared" si="2"/>
         <v>-384</v>
       </c>
-      <c r="J22" s="12">
+      <c r="J22" s="17">
         <f t="shared" si="2"/>
         <v>-290</v>
       </c>
-      <c r="K22" s="12">
+      <c r="K22" s="17">
         <f t="shared" si="2"/>
         <v>-255</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="17">
         <f t="shared" si="2"/>
         <v>-204</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M22" s="17">
         <f t="shared" si="2"/>
         <v>-176</v>
       </c>
-      <c r="N22" s="12">
+      <c r="N22" s="17">
         <f t="shared" si="2"/>
         <v>-93</v>
       </c>
-      <c r="O22" s="12">
+      <c r="O22" s="17">
         <f t="shared" si="2"/>
         <v>-46</v>
       </c>
-      <c r="P22" s="12">
+      <c r="P22" s="17">
         <f t="shared" si="2"/>
         <v>-75</v>
       </c>
-      <c r="Q22" s="12">
+      <c r="Q22" s="17">
         <f t="shared" si="2"/>
         <v>-6</v>
       </c>
-      <c r="R22" s="12">
+      <c r="R22" s="17">
         <f t="shared" si="2"/>
         <v>-38</v>
       </c>
-      <c r="S22" s="12">
+      <c r="S22" s="17">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="T22" s="12">
+      <c r="T22" s="17">
         <f>T16-SUM(T17:T21)</f>
         <v>-21</v>
       </c>
-      <c r="U22" s="12">
+      <c r="U22" s="17">
         <f>U16-SUM(U17:U21)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+      <c r="V22" s="17">
+        <f>V16-SUM(V17:V21)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="8">
         <v>-434</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="8">
         <v>-406</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="8">
         <v>-581</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="8">
         <v>-544</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="8">
         <v>12</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I23" s="8">
         <v>-185</v>
       </c>
-      <c r="J23" s="11">
+      <c r="J23" s="8">
         <v>-44</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K23" s="8">
         <v>-135</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="8">
         <v>-34</v>
       </c>
-      <c r="M23" s="11">
+      <c r="M23" s="8">
         <v>-25</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N23" s="8">
         <v>14</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="15">
         <v>54</v>
       </c>
-      <c r="P23" s="11">
+      <c r="P23" s="8">
         <v>-23</v>
       </c>
-      <c r="Q23" s="11">
+      <c r="Q23" s="8">
         <v>-5</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="15">
         <v>87</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="15">
         <v>12</v>
       </c>
-      <c r="T23">
+      <c r="T23" s="15">
         <v>45</v>
       </c>
-      <c r="U23">
+      <c r="U23" s="15">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="V23" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="11">
+      <c r="C24" s="2"/>
+      <c r="D24" s="8">
         <v>-665</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="8">
         <v>-799</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="8">
         <v>-984</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="8">
         <v>-1103</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="8">
         <v>-434</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I24" s="8">
         <v>-570</v>
       </c>
-      <c r="J24" s="11">
+      <c r="J24" s="8">
         <v>-338</v>
       </c>
-      <c r="K24" s="11">
+      <c r="K24" s="8">
         <v>-391</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="8">
         <v>-239</v>
       </c>
-      <c r="M24" s="11">
+      <c r="M24" s="8">
         <v>-153</v>
       </c>
-      <c r="N24" s="11">
+      <c r="N24" s="8">
         <v>-83</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="15">
         <v>7</v>
       </c>
-      <c r="P24" s="11">
+      <c r="P24" s="8">
         <v>-102</v>
       </c>
-      <c r="Q24" s="11">
+      <c r="Q24" s="8">
         <v>-51</v>
       </c>
-      <c r="R24" s="11">
+      <c r="R24" s="8">
         <v>47</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="15">
         <v>11</v>
       </c>
-      <c r="T24">
+      <c r="T24" s="15">
         <v>24</v>
       </c>
-      <c r="U24" s="11">
+      <c r="U24" s="8">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+      <c r="V24" s="8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="8">
         <v>1</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="8">
         <v>2</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F25" s="8">
         <v>4</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="8">
         <v>-3</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="8">
         <v>1</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I25" s="8">
         <v>2</v>
       </c>
-      <c r="J25" s="11">
+      <c r="J25" s="8">
         <v>4</v>
       </c>
-      <c r="K25" s="11">
+      <c r="K25" s="8">
         <v>0</v>
       </c>
-      <c r="L25" s="11">
+      <c r="L25" s="8">
         <v>11</v>
       </c>
-      <c r="M25" s="11">
+      <c r="M25" s="8">
         <v>-5</v>
       </c>
-      <c r="N25" s="11">
+      <c r="N25" s="8">
         <v>16</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="15">
         <v>-4</v>
       </c>
-      <c r="P25" s="11">
+      <c r="P25" s="8">
         <v>13</v>
       </c>
-      <c r="Q25" s="11">
+      <c r="Q25" s="8">
         <v>17</v>
       </c>
-      <c r="R25">
+      <c r="R25" s="15">
         <v>32</v>
       </c>
-      <c r="S25">
+      <c r="S25" s="15">
         <v>0</v>
       </c>
-      <c r="T25">
+      <c r="T25" s="15">
         <v>14</v>
       </c>
-      <c r="U25">
+      <c r="U25" s="15">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="18" t="s">
+      <c r="V25" s="15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="17">
         <f t="shared" ref="C26:S26" si="3">C24-C25</f>
         <v>0</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="17">
         <f t="shared" si="3"/>
         <v>-666</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="17">
         <f t="shared" si="3"/>
         <v>-801</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="17">
         <f t="shared" si="3"/>
         <v>-988</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="17">
         <f t="shared" si="3"/>
         <v>-1100</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="17">
         <f t="shared" si="3"/>
         <v>-435</v>
       </c>
-      <c r="I26" s="12">
+      <c r="I26" s="17">
         <f t="shared" si="3"/>
         <v>-572</v>
       </c>
-      <c r="J26" s="12">
+      <c r="J26" s="17">
         <f t="shared" si="3"/>
         <v>-342</v>
       </c>
-      <c r="K26" s="12">
+      <c r="K26" s="17">
         <f t="shared" si="3"/>
         <v>-391</v>
       </c>
-      <c r="L26" s="12">
+      <c r="L26" s="17">
         <f t="shared" si="3"/>
         <v>-250</v>
       </c>
-      <c r="M26" s="12">
+      <c r="M26" s="17">
         <f t="shared" si="3"/>
         <v>-148</v>
       </c>
-      <c r="N26" s="12">
+      <c r="N26" s="17">
         <f t="shared" si="3"/>
         <v>-99</v>
       </c>
-      <c r="O26" s="12">
+      <c r="O26" s="17">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="P26" s="12">
+      <c r="P26" s="17">
         <f t="shared" si="3"/>
         <v>-115</v>
       </c>
-      <c r="Q26" s="12">
+      <c r="Q26" s="17">
         <f t="shared" si="3"/>
         <v>-68</v>
       </c>
-      <c r="R26" s="12">
+      <c r="R26" s="17">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="S26" s="12">
+      <c r="S26" s="17">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="T26" s="12">
+      <c r="T26" s="17">
         <f>T24-T25</f>
         <v>10</v>
       </c>
-      <c r="U26" s="12">
+      <c r="U26" s="17">
         <f>U24-U25</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="19" t="s">
+      <c r="V26" s="17">
+        <f>V24-V25</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="20">
         <v>-111</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="20">
         <v>-214</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="20">
         <v>-212</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="20">
         <v>-305</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="20">
         <v>-287</v>
       </c>
-      <c r="I27" s="8">
+      <c r="I27" s="20">
         <v>-233</v>
       </c>
-      <c r="J27" s="8">
+      <c r="J27" s="20">
         <v>-161</v>
       </c>
-      <c r="K27" s="8">
+      <c r="K27" s="20">
         <v>-111</v>
       </c>
-      <c r="L27" s="8">
+      <c r="L27" s="20">
         <v>-67</v>
       </c>
-      <c r="M27" s="8">
+      <c r="M27" s="20">
         <v>-17</v>
       </c>
       <c r="N27" s="21">
@@ -2947,466 +3095,485 @@
       <c r="T27" s="21">
         <v>106</v>
       </c>
-      <c r="U27" s="35">
+      <c r="U27" s="22">
         <v>109</v>
       </c>
-      <c r="V27" s="23">
-        <f xml:space="preserve"> U27 * 1.07</f>
-        <v>116.63000000000001</v>
-      </c>
-      <c r="W27" s="23">
+      <c r="V27" s="19">
+        <v>136</v>
+      </c>
+      <c r="W27" s="19">
         <f xml:space="preserve"> V27 * 1.07</f>
-        <v>124.79410000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
+        <v>145.52000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4">
         <v>-3.18</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="4">
         <v>-2.89</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="4">
         <v>-3.66</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="4">
         <v>-0.74</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="4">
         <v>-0.11</v>
       </c>
-      <c r="I28" s="5">
+      <c r="I28" s="4">
         <v>-0.15</v>
       </c>
-      <c r="J28" s="5">
+      <c r="J28" s="4">
         <v>-0.08</v>
       </c>
-      <c r="K28" s="5">
+      <c r="K28" s="4">
         <v>-0.1</v>
       </c>
-      <c r="L28" s="5">
+      <c r="L28" s="4">
         <v>-0.06</v>
       </c>
-      <c r="M28" s="5">
+      <c r="M28" s="4">
         <v>-0.03</v>
       </c>
-      <c r="N28" s="5">
+      <c r="N28" s="4">
         <v>-0.02</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="15">
         <v>0.01</v>
       </c>
-      <c r="P28" s="5">
+      <c r="P28" s="4">
         <v>-0.03</v>
       </c>
-      <c r="Q28" s="5">
+      <c r="Q28" s="4">
         <v>-0.01</v>
       </c>
-      <c r="R28" s="5">
+      <c r="R28" s="4">
         <v>0.01</v>
       </c>
-      <c r="S28" s="5">
+      <c r="S28" s="4">
         <v>0.01</v>
       </c>
-      <c r="T28">
+      <c r="T28" s="15">
         <v>0.01</v>
       </c>
-      <c r="U28" s="5">
+      <c r="U28" s="4">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
+      <c r="V28" s="4">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1">
         <v>-3.18</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="1">
         <v>-2.89</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="1">
         <v>-3.66</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="1">
         <v>-0.74</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="1">
         <v>-0.11</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="1">
         <v>-0.15</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="1">
         <v>-0.08</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="1">
         <v>-0.1</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L29" s="1">
         <v>-0.06</v>
       </c>
-      <c r="M29" s="11">
+      <c r="M29" s="8">
         <v>-0.03</v>
       </c>
-      <c r="N29" s="11">
+      <c r="N29" s="8">
         <v>-0.02</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="15">
         <v>0.01</v>
       </c>
-      <c r="P29" s="11">
+      <c r="P29" s="8">
         <v>-0.03</v>
       </c>
-      <c r="Q29" s="11">
+      <c r="Q29" s="8">
         <v>-0.01</v>
       </c>
-      <c r="R29">
+      <c r="R29" s="15">
         <v>0.01</v>
       </c>
-      <c r="S29">
+      <c r="S29" s="15">
         <v>0.01</v>
       </c>
-      <c r="T29">
+      <c r="T29" s="15">
         <v>0.01</v>
       </c>
-      <c r="U29">
+      <c r="U29" s="15">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+      <c r="V29" s="15">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14">
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24">
         <f t="shared" ref="H31:S31" si="4">(H13/D13) - 1</f>
         <v>5.555555555555558E-2</v>
       </c>
-      <c r="I31" s="14">
+      <c r="I31" s="24">
         <f t="shared" si="4"/>
         <v>0.7932960893854748</v>
       </c>
-      <c r="J31" s="14">
+      <c r="J31" s="24">
         <f t="shared" si="4"/>
         <v>1.4331210191082802</v>
       </c>
-      <c r="K31" s="14">
+      <c r="K31" s="24">
         <f t="shared" si="4"/>
         <v>3.1147540983606561</v>
       </c>
-      <c r="L31" s="14">
+      <c r="L31" s="24">
         <f t="shared" si="4"/>
         <v>1.3026315789473686</v>
       </c>
-      <c r="M31" s="14">
+      <c r="M31" s="24">
         <f t="shared" si="4"/>
         <v>0.76635514018691597</v>
       </c>
-      <c r="N31" s="14">
+      <c r="N31" s="24">
         <f t="shared" si="4"/>
         <v>0.60994764397905765</v>
       </c>
-      <c r="O31" s="14">
+      <c r="O31" s="24">
         <f t="shared" si="4"/>
         <v>0.30079681274900394</v>
       </c>
-      <c r="P31" s="14">
+      <c r="P31" s="24">
         <f t="shared" si="4"/>
         <v>0.24380952380952392</v>
       </c>
-      <c r="Q31" s="14">
+      <c r="Q31" s="24">
         <f t="shared" si="4"/>
         <v>0.17107583774250434</v>
       </c>
-      <c r="R31" s="14">
+      <c r="R31" s="24">
         <f t="shared" si="4"/>
         <v>0.16422764227642284</v>
       </c>
-      <c r="S31" s="14">
+      <c r="S31" s="24">
         <f t="shared" si="4"/>
         <v>0.1699846860643186</v>
       </c>
-      <c r="T31" s="14">
+      <c r="T31" s="24">
         <f>(T13/P13) - 1</f>
         <v>0.18376722817764168</v>
       </c>
-      <c r="U31" s="14">
+      <c r="U31" s="24">
         <f>(U13/Q13) - 1</f>
         <v>0.23343373493975905</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+      <c r="V31" s="24">
+        <f>(V13/R13) - 1</f>
+        <v>0.21927374301675973</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14">
+      <c r="D32" s="24"/>
+      <c r="E32" s="24">
         <f t="shared" ref="E32:G32" si="5" xml:space="preserve"> (E13/D13) - 1</f>
         <v>-0.17129629629629628</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="24">
         <f t="shared" si="5"/>
         <v>-0.12290502793296088</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="24">
         <f t="shared" si="5"/>
         <v>-0.22292993630573243</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="24">
         <f t="shared" ref="H32:S32" si="6" xml:space="preserve"> (H13/G13) - 1</f>
         <v>0.86885245901639352</v>
       </c>
-      <c r="I32" s="14">
+      <c r="I32" s="24">
         <f t="shared" si="6"/>
         <v>0.40789473684210531</v>
       </c>
-      <c r="J32" s="14">
+      <c r="J32" s="24">
         <f t="shared" si="6"/>
         <v>0.19003115264797499</v>
       </c>
-      <c r="K32" s="14">
+      <c r="K32" s="24">
         <f t="shared" si="6"/>
         <v>0.31413612565445037</v>
       </c>
-      <c r="L32" s="14">
+      <c r="L32" s="24">
         <f t="shared" si="6"/>
         <v>4.5816733067729043E-2</v>
       </c>
-      <c r="M32" s="14">
+      <c r="M32" s="24">
         <f t="shared" si="6"/>
         <v>8.0000000000000071E-2</v>
       </c>
-      <c r="N32" s="14">
+      <c r="N32" s="24">
         <f t="shared" si="6"/>
         <v>8.4656084656084651E-2</v>
       </c>
-      <c r="O32" s="14">
+      <c r="O32" s="24">
         <f t="shared" si="6"/>
         <v>6.1788617886178843E-2</v>
       </c>
-      <c r="P32" s="14">
+      <c r="P32" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Q32" s="14">
+      <c r="Q32" s="24">
         <f t="shared" si="6"/>
         <v>1.6845329249617125E-2</v>
       </c>
-      <c r="R32" s="14">
+      <c r="R32" s="24">
         <f t="shared" si="6"/>
         <v>7.8313253012048278E-2</v>
       </c>
-      <c r="S32" s="14">
+      <c r="S32" s="24">
         <f t="shared" si="6"/>
         <v>6.7039106145251326E-2</v>
       </c>
-      <c r="T32" s="14">
+      <c r="T32" s="24">
         <f xml:space="preserve"> (T13/S13) - 1</f>
         <v>1.1780104712041828E-2</v>
       </c>
-      <c r="U32" s="14">
+      <c r="U32" s="24">
         <f xml:space="preserve"> (U13/T13) - 1</f>
         <v>5.9508408796895118E-2</v>
       </c>
-    </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="16"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="16"/>
-      <c r="T33" s="14"/>
-    </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
-      <c r="O34" s="16"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="16"/>
-      <c r="T34" s="14"/>
-    </row>
-    <row r="36" spans="2:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+      <c r="V32" s="24">
+        <f xml:space="preserve"> (V13/U13) - 1</f>
+        <v>6.5934065934065922E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26"/>
+      <c r="Q33" s="26"/>
+      <c r="R33" s="26"/>
+      <c r="S33" s="26"/>
+      <c r="T33" s="25"/>
+    </row>
+    <row r="34" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B34" s="1"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="26"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="26"/>
+      <c r="P34" s="26"/>
+      <c r="Q34" s="26"/>
+      <c r="R34" s="26"/>
+      <c r="S34" s="26"/>
+      <c r="T34" s="25"/>
+    </row>
+    <row r="36" spans="2:30" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="10">
+      <c r="C36" s="3"/>
+      <c r="D36" s="7">
         <v>-434</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="7">
         <v>-799</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F36" s="7">
         <v>-984</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G36" s="7">
         <v>-1103</v>
       </c>
-      <c r="H36" s="10">
+      <c r="H36" s="7">
         <v>-665</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I36" s="7">
         <v>-570</v>
       </c>
-      <c r="J36" s="10">
+      <c r="J36" s="7">
         <v>-338</v>
       </c>
-      <c r="K36" s="10">
+      <c r="K36" s="7">
         <v>-391</v>
       </c>
-      <c r="L36" s="10">
+      <c r="L36" s="7">
         <v>-11</v>
       </c>
-      <c r="M36" s="10">
+      <c r="M36" s="7">
         <v>-51</v>
       </c>
-      <c r="N36" s="10">
+      <c r="N36" s="7">
         <v>322</v>
       </c>
-      <c r="O36" s="10">
+      <c r="O36" s="7">
         <v>-26</v>
       </c>
-      <c r="P36" s="10">
+      <c r="P36" s="7">
         <v>-11</v>
       </c>
-      <c r="Q36" s="8">
+      <c r="Q36" s="20">
         <v>272</v>
       </c>
-      <c r="R36" s="8">
+      <c r="R36" s="20">
         <v>338</v>
       </c>
-      <c r="S36" s="8">
+      <c r="S36" s="20">
         <v>253</v>
       </c>
-      <c r="T36" s="8">
+      <c r="T36" s="20">
         <v>73</v>
       </c>
-      <c r="U36" s="8">
+      <c r="U36" s="20">
         <v>64</v>
       </c>
-    </row>
-    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
+      <c r="V36" s="20">
+        <v>-127</v>
+      </c>
+    </row>
+    <row r="37" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B37" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11">
+      <c r="C37" s="2"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8">
         <v>22</v>
       </c>
-      <c r="M37" s="11">
+      <c r="M37" s="8">
         <v>34</v>
       </c>
-      <c r="N37" s="11">
+      <c r="N37" s="8">
         <v>47</v>
       </c>
-      <c r="O37" s="11">
+      <c r="O37" s="8">
         <v>38</v>
       </c>
-      <c r="P37" s="11">
+      <c r="P37" s="8">
         <v>14</v>
       </c>
-      <c r="Q37" s="11">
+      <c r="Q37" s="8">
         <v>27</v>
       </c>
-      <c r="R37">
+      <c r="R37" s="15">
         <v>46</v>
       </c>
-      <c r="S37">
+      <c r="S37" s="15">
         <v>53</v>
       </c>
-      <c r="T37">
+      <c r="T37" s="15">
         <v>35</v>
       </c>
-      <c r="U37">
+      <c r="U37" s="15">
         <v>25</v>
       </c>
-    </row>
-    <row r="38" spans="2:30" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="17" t="s">
+      <c r="V37" s="15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="2:30" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B38" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="17">
         <f t="shared" ref="C38:S38" si="7">C36-C37</f>
         <v>0</v>
       </c>
-      <c r="D38" s="12">
+      <c r="D38" s="17">
         <f t="shared" si="7"/>
         <v>-434</v>
       </c>
-      <c r="E38" s="12">
+      <c r="E38" s="17">
         <f t="shared" si="7"/>
         <v>-799</v>
       </c>
-      <c r="F38" s="12">
+      <c r="F38" s="17">
         <f t="shared" si="7"/>
         <v>-984</v>
       </c>
-      <c r="G38" s="12">
+      <c r="G38" s="17">
         <f t="shared" si="7"/>
         <v>-1103</v>
       </c>
-      <c r="H38" s="12">
+      <c r="H38" s="17">
         <f t="shared" si="7"/>
         <v>-665</v>
       </c>
-      <c r="I38" s="12">
+      <c r="I38" s="17">
         <f t="shared" si="7"/>
         <v>-570</v>
       </c>
-      <c r="J38" s="12">
+      <c r="J38" s="17">
         <f t="shared" si="7"/>
         <v>-338</v>
       </c>
-      <c r="K38" s="12">
+      <c r="K38" s="17">
         <f t="shared" si="7"/>
         <v>-391</v>
       </c>
-      <c r="L38" s="12">
+      <c r="L38" s="17">
         <f t="shared" si="7"/>
         <v>-33</v>
       </c>
-      <c r="M38" s="12">
+      <c r="M38" s="17">
         <f t="shared" si="7"/>
         <v>-85</v>
       </c>
@@ -3442,404 +3609,411 @@
         <f>U36-U37</f>
         <v>39</v>
       </c>
-    </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-    </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
+      <c r="V38" s="21">
+        <f>V36-V37</f>
+        <v>-154</v>
+      </c>
+    </row>
+    <row r="39" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B39" s="2"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+    </row>
+    <row r="40" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B40" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H40" s="14">
+      <c r="H40" s="25">
         <f t="shared" ref="H40:S40" si="8">IF(D38=0,IF(H38=0,0,NA()),(H38-D38)/ABS(D38))</f>
         <v>-0.532258064516129</v>
       </c>
-      <c r="I40" s="14">
+      <c r="I40" s="25">
         <f t="shared" si="8"/>
         <v>0.28660826032540676</v>
       </c>
-      <c r="J40" s="14">
+      <c r="J40" s="25">
         <f t="shared" si="8"/>
         <v>0.6565040650406504</v>
       </c>
-      <c r="K40" s="14">
+      <c r="K40" s="25">
         <f t="shared" si="8"/>
         <v>0.64551223934723478</v>
       </c>
-      <c r="L40" s="14">
+      <c r="L40" s="25">
         <f t="shared" si="8"/>
         <v>0.9503759398496241</v>
       </c>
-      <c r="M40" s="14">
+      <c r="M40" s="25">
         <f t="shared" si="8"/>
         <v>0.85087719298245612</v>
       </c>
-      <c r="N40" s="14">
+      <c r="N40" s="25">
         <f t="shared" si="8"/>
         <v>1.8136094674556213</v>
       </c>
-      <c r="O40" s="14">
+      <c r="O40" s="25">
         <f t="shared" si="8"/>
         <v>0.83631713554987208</v>
       </c>
-      <c r="P40" s="14">
+      <c r="P40" s="25">
         <f t="shared" si="8"/>
         <v>0.24242424242424243</v>
       </c>
-      <c r="Q40" s="14">
+      <c r="Q40" s="25">
         <f t="shared" si="8"/>
         <v>3.8823529411764706</v>
       </c>
-      <c r="R40" s="14">
+      <c r="R40" s="25">
         <f t="shared" si="8"/>
         <v>6.1818181818181821E-2</v>
       </c>
-      <c r="S40" s="14">
+      <c r="S40" s="25">
         <f t="shared" si="8"/>
         <v>4.125</v>
       </c>
-      <c r="T40" s="14">
+      <c r="T40" s="25">
         <f>IF(P38=0,IF(T38=0,0,NA()),(T38-P38)/ABS(P38))</f>
         <v>2.52</v>
       </c>
-      <c r="U40" s="14">
+      <c r="U40" s="25">
         <f>IF(Q38=0,IF(U38=0,0,NA()),(U38-Q38)/ABS(Q38))</f>
         <v>-0.84081632653061222</v>
       </c>
     </row>
-    <row r="42" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="3"/>
-      <c r="D42" s="15"/>
-      <c r="K42" s="15"/>
-    </row>
-    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+    <row r="42" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
+      <c r="D42" s="27"/>
+      <c r="K42" s="27"/>
+    </row>
+    <row r="43" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B43" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="25"/>
-      <c r="N43" s="25"/>
-      <c r="O43" s="25"/>
-      <c r="P43" s="25"/>
-      <c r="Q43" s="25"/>
-      <c r="R43" s="25"/>
-      <c r="S43" s="32" t="s">
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="T43" s="25" t="s">
+      <c r="T43" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="U43" s="34">
+      <c r="U43" s="31">
         <f>SUM(T13:W13)</f>
-        <v>3354.8975</v>
-      </c>
-      <c r="V43" s="25" t="s">
+        <v>3381.65</v>
+      </c>
+      <c r="V43" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="W43" s="25"/>
-      <c r="X43" s="25"/>
-      <c r="Y43" s="25"/>
-      <c r="Z43" s="25"/>
-      <c r="AA43" s="25"/>
-      <c r="AB43" s="25"/>
-      <c r="AC43" s="25"/>
-      <c r="AD43" s="26"/>
-    </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B44" s="27"/>
-      <c r="S44" t="s">
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="29"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="32"/>
+    </row>
+    <row r="44" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B44" s="33"/>
+      <c r="S44" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="T44" t="s">
+      <c r="T44" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="U44" t="s">
+      <c r="U44" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="AD44" s="28"/>
-    </row>
-    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B45" s="27"/>
-      <c r="S45" t="s">
+      <c r="AD44" s="35"/>
+    </row>
+    <row r="45" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B45" s="33"/>
+      <c r="S45" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="T45" t="s">
+      <c r="T45" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="U45" s="33">
+      <c r="U45" s="36">
         <f xml:space="preserve"> SUM(T27:W27)</f>
-        <v>456.42410000000001</v>
-      </c>
-      <c r="AD45" s="28"/>
-    </row>
-    <row r="46" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="29"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
-      <c r="K46" s="30"/>
-      <c r="L46" s="30"/>
-      <c r="M46" s="30"/>
-      <c r="N46" s="30"/>
-      <c r="O46" s="30"/>
-      <c r="P46" s="30"/>
-      <c r="Q46" s="30"/>
-      <c r="R46" s="30"/>
-      <c r="S46" s="30"/>
-      <c r="T46" s="30" t="s">
+        <v>496.52</v>
+      </c>
+      <c r="V45" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD45" s="35"/>
+    </row>
+    <row r="46" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="37"/>
+      <c r="C46" s="38"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
+      <c r="K46" s="38"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="38"/>
+      <c r="N46" s="38"/>
+      <c r="O46" s="38"/>
+      <c r="P46" s="38"/>
+      <c r="Q46" s="38"/>
+      <c r="R46" s="38"/>
+      <c r="S46" s="38"/>
+      <c r="T46" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="U46" s="30" t="s">
+      <c r="U46" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="V46" s="30"/>
-      <c r="W46" s="30"/>
-      <c r="X46" s="30"/>
-      <c r="Y46" s="30"/>
-      <c r="Z46" s="30"/>
-      <c r="AA46" s="30"/>
-      <c r="AB46" s="30"/>
-      <c r="AC46" s="30"/>
-      <c r="AD46" s="31"/>
-    </row>
-    <row r="47" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B48" s="24" t="s">
+      <c r="V46" s="38"/>
+      <c r="W46" s="38"/>
+      <c r="X46" s="38"/>
+      <c r="Y46" s="38"/>
+      <c r="Z46" s="38"/>
+      <c r="AA46" s="38"/>
+      <c r="AB46" s="38"/>
+      <c r="AC46" s="38"/>
+      <c r="AD46" s="40"/>
+    </row>
+    <row r="47" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B48" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25" t="s">
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="25"/>
-      <c r="N48" s="25"/>
-      <c r="O48" s="25"/>
-      <c r="P48" s="25"/>
-      <c r="Q48" s="25" t="s">
+      <c r="I48" s="29"/>
+      <c r="J48" s="29"/>
+      <c r="K48" s="29"/>
+      <c r="L48" s="29"/>
+      <c r="M48" s="29"/>
+      <c r="N48" s="29"/>
+      <c r="O48" s="29"/>
+      <c r="P48" s="29"/>
+      <c r="Q48" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="R48" s="25"/>
-      <c r="S48" s="25"/>
-      <c r="T48" s="25" t="s">
+      <c r="R48" s="29"/>
+      <c r="S48" s="29"/>
+      <c r="T48" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="U48" s="25"/>
-      <c r="V48" s="25"/>
-      <c r="W48" s="26"/>
-    </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B49" s="27"/>
-      <c r="I49" t="s">
+      <c r="U48" s="29"/>
+      <c r="V48" s="29"/>
+      <c r="W48" s="32"/>
+    </row>
+    <row r="49" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B49" s="33"/>
+      <c r="I49" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="T49" t="s">
+      <c r="T49" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="W49" s="28"/>
-    </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B50" s="27"/>
-      <c r="J50" t="s">
+      <c r="W49" s="35"/>
+    </row>
+    <row r="50" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B50" s="33"/>
+      <c r="J50" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="T50" t="s">
+      <c r="T50" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="W50" s="28"/>
-    </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B51" s="27"/>
-      <c r="N51" t="s">
+      <c r="W50" s="35"/>
+    </row>
+    <row r="51" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B51" s="33"/>
+      <c r="N51" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="W51" s="28"/>
-    </row>
-    <row r="52" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="29"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
-      <c r="G52" s="30"/>
-      <c r="H52" s="30"/>
-      <c r="I52" s="30"/>
-      <c r="J52" s="30"/>
-      <c r="K52" s="30"/>
-      <c r="L52" s="30"/>
-      <c r="M52" s="30"/>
-      <c r="N52" s="30" t="s">
+      <c r="W51" s="35"/>
+    </row>
+    <row r="52" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="37"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="38"/>
+      <c r="K52" s="38"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="38"/>
+      <c r="N52" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="O52" s="30"/>
-      <c r="P52" s="30"/>
-      <c r="Q52" s="30"/>
-      <c r="R52" s="30"/>
-      <c r="S52" s="30"/>
-      <c r="T52" s="30"/>
-      <c r="U52" s="30"/>
-      <c r="V52" s="30"/>
-      <c r="W52" s="31"/>
-    </row>
-    <row r="53" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B54" s="24" t="s">
+      <c r="O52" s="38"/>
+      <c r="P52" s="38"/>
+      <c r="Q52" s="38"/>
+      <c r="R52" s="38"/>
+      <c r="S52" s="38"/>
+      <c r="T52" s="38"/>
+      <c r="U52" s="38"/>
+      <c r="V52" s="38"/>
+      <c r="W52" s="40"/>
+    </row>
+    <row r="53" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B54" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="25" t="s">
+      <c r="C54" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D54" s="25"/>
-      <c r="E54" s="26"/>
-    </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B55" s="27"/>
-      <c r="C55" t="s">
+      <c r="D54" s="29"/>
+      <c r="E54" s="32"/>
+    </row>
+    <row r="55" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B55" s="33"/>
+      <c r="C55" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E55" s="28"/>
-    </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B56" s="27"/>
-      <c r="C56" t="s">
+      <c r="E55" s="35"/>
+    </row>
+    <row r="56" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B56" s="33"/>
+      <c r="C56" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E56" s="28"/>
-    </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B57" s="27"/>
-      <c r="C57" t="s">
+      <c r="E56" s="35"/>
+    </row>
+    <row r="57" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B57" s="33"/>
+      <c r="C57" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E57" s="28"/>
-    </row>
-    <row r="58" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="29"/>
-      <c r="C58" s="30" t="s">
+      <c r="E57" s="35"/>
+    </row>
+    <row r="58" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="37"/>
+      <c r="C58" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="D58" s="30"/>
-      <c r="E58" s="31"/>
-    </row>
-    <row r="59" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B60" s="24" t="s">
+      <c r="D58" s="38"/>
+      <c r="E58" s="40"/>
+    </row>
+    <row r="59" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B60" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
-      <c r="I60" s="25"/>
-      <c r="J60" s="25"/>
-      <c r="K60" s="25"/>
-      <c r="L60" s="25"/>
-      <c r="M60" s="25"/>
-      <c r="N60" s="25"/>
-      <c r="O60" s="25"/>
-      <c r="P60" s="26"/>
-    </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B61" s="27"/>
-      <c r="C61" t="s">
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="29"/>
+      <c r="L60" s="29"/>
+      <c r="M60" s="29"/>
+      <c r="N60" s="29"/>
+      <c r="O60" s="29"/>
+      <c r="P60" s="32"/>
+    </row>
+    <row r="61" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B61" s="33"/>
+      <c r="C61" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="P61" s="28"/>
-    </row>
-    <row r="62" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B62" s="27"/>
-      <c r="P62" s="28"/>
-    </row>
-    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B63" s="27"/>
-      <c r="C63" t="s">
+      <c r="P61" s="35"/>
+    </row>
+    <row r="62" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B62" s="33"/>
+      <c r="P62" s="35"/>
+    </row>
+    <row r="63" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B63" s="33"/>
+      <c r="C63" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="P63" s="28"/>
-    </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B64" s="27"/>
-      <c r="P64" s="28"/>
-    </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B65" s="27"/>
-      <c r="C65" t="s">
+      <c r="P63" s="35"/>
+    </row>
+    <row r="64" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B64" s="33"/>
+      <c r="P64" s="35"/>
+    </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B65" s="33"/>
+      <c r="C65" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="P65" s="28"/>
-    </row>
-    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B66" s="27"/>
-      <c r="P66" s="28"/>
-    </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B67" s="27"/>
-      <c r="P67" s="28"/>
-    </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B68" s="27"/>
-      <c r="P68" s="28"/>
-    </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B69" s="27"/>
-      <c r="P69" s="28"/>
-    </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B70" s="27"/>
-      <c r="P70" s="28"/>
-    </row>
-    <row r="71" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="29"/>
-      <c r="C71" s="30"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="30"/>
-      <c r="G71" s="30"/>
-      <c r="H71" s="30"/>
-      <c r="I71" s="30"/>
-      <c r="J71" s="30"/>
-      <c r="K71" s="30"/>
-      <c r="L71" s="30"/>
-      <c r="M71" s="30"/>
-      <c r="N71" s="30"/>
-      <c r="O71" s="30"/>
-      <c r="P71" s="31"/>
+      <c r="P65" s="35"/>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B66" s="33"/>
+      <c r="P66" s="35"/>
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B67" s="33"/>
+      <c r="P67" s="35"/>
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B68" s="33"/>
+      <c r="P68" s="35"/>
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B69" s="33"/>
+      <c r="P69" s="35"/>
+    </row>
+    <row r="70" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B70" s="33"/>
+      <c r="P70" s="35"/>
+    </row>
+    <row r="71" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="37"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
+      <c r="I71" s="38"/>
+      <c r="J71" s="38"/>
+      <c r="K71" s="38"/>
+      <c r="L71" s="38"/>
+      <c r="M71" s="38"/>
+      <c r="N71" s="38"/>
+      <c r="O71" s="38"/>
+      <c r="P71" s="40"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3856,50 +4030,51 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="13">
+      <c r="B1" s="41">
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="41">
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="41">
         <v>1500</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3913,7 +4088,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W31" sqref="W31"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3927,8 +4102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EFDD79E-6889-434B-8DF5-399E48D56148}">
   <dimension ref="A35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3945,6 +4120,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C341BEE4C9A91F44BB4A4EF8E0A71E02" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db93f7cdcc50be3ddb7642c8d50e9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="878aac0c-df32-40a9-a231-d93e9c7b9b1a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b63aaf3684aa43c37ed0cc1f5c2cf36e" ns3:_="">
     <xsd:import namespace="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
@@ -4088,22 +4278,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D65B96D-4012-4621-9665-52F685045C2D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9D266F6-4EBB-4FCE-8CE5-50B9641EB015}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4119,28 +4318,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D65B96D-4012-4621-9665-52F685045C2D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>